<commit_message>
Uploading trees and multiple sequence alignments for those including ECIV sequences (newly added to analysis).
</commit_message>
<xml_diff>
--- a/gene_review.xlsx
+++ b/gene_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="870" documentId="8_{6055D0A3-676A-4D4D-A9E1-9A76BC3762E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0141E717-108E-44DD-B5FD-A50BAA159885}"/>
+  <xr:revisionPtr revIDLastSave="877" documentId="8_{6055D0A3-676A-4D4D-A9E1-9A76BC3762E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E392C42-2129-4252-B1F8-3066573398AD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F9A2E0A-FCD5-4099-AB1E-88BFB846A76D}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6F9A2E0A-FCD5-4099-AB1E-88BFB846A76D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1144,10 +1144,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFB773-84C8-4FDF-A3F8-2F632CD15839}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,7 +1394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1507,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2229,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2511,7 +2512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>36</v>
       </c>
@@ -2719,7 +2720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
         <v>44</v>
       </c>
@@ -2771,7 +2772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
         <v>46</v>
       </c>
@@ -2875,7 +2876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
         <v>50</v>
       </c>
@@ -2901,7 +2902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
         <v>51</v>
       </c>
@@ -2979,7 +2980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
         <v>54</v>
       </c>
@@ -3057,7 +3058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
         <v>57</v>
       </c>
@@ -3083,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
         <v>58</v>
       </c>
@@ -3109,7 +3110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
         <v>59</v>
       </c>
@@ -3187,7 +3188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
         <v>62</v>
       </c>
@@ -3213,7 +3214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
         <v>63</v>
       </c>
@@ -3239,7 +3240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E66" t="s">
         <v>64</v>
       </c>
@@ -3265,7 +3266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E67" t="s">
         <v>65</v>
       </c>
@@ -3317,7 +3318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
         <v>67</v>
       </c>
@@ -3343,7 +3344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
         <v>68</v>
       </c>
@@ -3395,7 +3396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
         <v>70</v>
       </c>
@@ -3421,7 +3422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
         <v>71</v>
       </c>
@@ -3447,7 +3448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
         <v>72</v>
       </c>
@@ -3473,7 +3474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
         <v>73</v>
       </c>
@@ -3499,7 +3500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
         <v>74</v>
       </c>
@@ -3525,7 +3526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
         <v>75</v>
       </c>
@@ -3551,7 +3552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
         <v>76</v>
       </c>
@@ -3577,7 +3578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
         <v>77</v>
       </c>
@@ -3603,7 +3604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E80" t="s">
         <v>78</v>
       </c>
@@ -3629,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E81" t="s">
         <v>79</v>
       </c>
@@ -3655,7 +3656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E82" t="s">
         <v>80</v>
       </c>
@@ -3681,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E83" t="s">
         <v>81</v>
       </c>
@@ -3707,7 +3708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E84" t="s">
         <v>82</v>
       </c>
@@ -3733,7 +3734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E85" t="s">
         <v>83</v>
       </c>
@@ -3759,7 +3760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E86" t="s">
         <v>84</v>
       </c>
@@ -3785,7 +3786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E87" t="s">
         <v>85</v>
       </c>
@@ -3811,7 +3812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E88" t="s">
         <v>86</v>
       </c>
@@ -3837,7 +3838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E89" t="s">
         <v>87</v>
       </c>
@@ -3863,7 +3864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E90" t="s">
         <v>88</v>
       </c>
@@ -3889,7 +3890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E91" t="s">
         <v>89</v>
       </c>
@@ -3915,7 +3916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E92" t="s">
         <v>90</v>
       </c>
@@ -3941,7 +3942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E93" t="s">
         <v>91</v>
       </c>
@@ -3967,7 +3968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E94" t="s">
         <v>92</v>
       </c>
@@ -3993,7 +3994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E95" t="s">
         <v>93</v>
       </c>
@@ -4019,7 +4020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E96" t="s">
         <v>94</v>
       </c>
@@ -4045,7 +4046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E97" t="s">
         <v>95</v>
       </c>
@@ -4071,7 +4072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E98" t="s">
         <v>96</v>
       </c>
@@ -4097,7 +4098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E99" t="s">
         <v>97</v>
       </c>
@@ -4123,7 +4124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E100" t="s">
         <v>98</v>
       </c>
@@ -4149,7 +4150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E101" t="s">
         <v>99</v>
       </c>
@@ -4175,7 +4176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E102" t="s">
         <v>100</v>
       </c>
@@ -4201,7 +4202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E103" t="s">
         <v>101</v>
       </c>
@@ -4227,7 +4228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E104" t="s">
         <v>102</v>
       </c>
@@ -4253,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E105" t="s">
         <v>103</v>
       </c>
@@ -4279,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E106" t="s">
         <v>104</v>
       </c>
@@ -4305,7 +4306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E107" t="s">
         <v>105</v>
       </c>
@@ -4331,7 +4332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E108" t="s">
         <v>106</v>
       </c>
@@ -4357,7 +4358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E109" t="s">
         <v>107</v>
       </c>
@@ -4383,7 +4384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E110" t="s">
         <v>108</v>
       </c>
@@ -4435,7 +4436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E112" t="s">
         <v>110</v>
       </c>
@@ -4461,7 +4462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E113" t="s">
         <v>111</v>
       </c>
@@ -4487,7 +4488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E114" t="s">
         <v>112</v>
       </c>
@@ -4513,7 +4514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E115" t="s">
         <v>113</v>
       </c>
@@ -4539,7 +4540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E116" t="s">
         <v>114</v>
       </c>
@@ -4566,7 +4567,23 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L116" xr:uid="{A9EFB773-84C8-4FDF-A3F8-2F632CD15839}"/>
+  <autoFilter ref="A1:L116" xr:uid="{A9EFB773-84C8-4FDF-A3F8-2F632CD15839}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="7">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B1:D1048576">
     <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">

</xml_diff>

<commit_message>
Updates genes for concatenation after removing and adding genes which should / should not have been included in the last collection.
</commit_message>
<xml_diff>
--- a/gene_review.xlsx
+++ b/gene_review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1276" documentId="8_{6055D0A3-676A-4D4D-A9E1-9A76BC3762E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E572F42-0206-4C0A-AE8D-431CF9158EF8}"/>
+  <xr:revisionPtr revIDLastSave="1287" documentId="8_{6055D0A3-676A-4D4D-A9E1-9A76BC3762E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5782BA60-01A3-41AC-8D1A-56A641618F53}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9960" xr2:uid="{6F9A2E0A-FCD5-4099-AB1E-88BFB846A76D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6F9A2E0A-FCD5-4099-AB1E-88BFB846A76D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -867,13 +867,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFB773-84C8-4FDF-A3F8-2F632CD15839}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="H114" sqref="H114"/>
+    <sheetView tabSelected="1" topLeftCell="F72" zoomScale="95" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="L117" sqref="L4:L117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -930,7 +930,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -968,7 +968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E33" t="s">
         <v>31</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E34" t="s">
         <v>32</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E35" t="s">
         <v>33</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E36" t="s">
         <v>34</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E37" t="s">
         <v>35</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E38" t="s">
         <v>36</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E39" t="s">
         <v>37</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E40" t="s">
         <v>38</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E41" t="s">
         <v>39</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E42" t="s">
         <v>40</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E45" t="s">
         <v>43</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E46" t="s">
         <v>44</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E47" t="s">
         <v>45</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E48" t="s">
         <v>46</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E52" t="s">
         <v>50</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E54" t="s">
         <v>52</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E55" t="s">
         <v>53</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E56" t="s">
         <v>54</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E57" t="s">
         <v>55</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E60" t="s">
         <v>58</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E84" t="s">
         <v>82</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="89" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E89" t="s">
         <v>87</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E93" t="s">
         <v>91</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E96" t="s">
         <v>94</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E97" t="s">
         <v>95</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E98" t="s">
         <v>96</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E100" t="s">
         <v>98</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E101" t="s">
         <v>99</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E102" t="s">
         <v>100</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E107" t="s">
         <v>105</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E108" t="s">
         <v>106</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="110" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E110" t="s">
         <v>108</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="114" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E114" t="s">
         <v>112</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E115" t="s">
         <v>113</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="E116" t="s">
         <v>114</v>
       </c>
@@ -4319,7 +4319,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L117" xr:uid="{A9EFB773-84C8-4FDF-A3F8-2F632CD15839}"/>
+  <autoFilter ref="A1:L117" xr:uid="{A9EFB773-84C8-4FDF-A3F8-2F632CD15839}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B1:D1048576">
     <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">

</xml_diff>

<commit_message>
Uploading iqtree outputs from latest iqtree tun to generate final trees.
</commit_message>
<xml_diff>
--- a/gene_review.xlsx
+++ b/gene_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1287" documentId="8_{6055D0A3-676A-4D4D-A9E1-9A76BC3762E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5782BA60-01A3-41AC-8D1A-56A641618F53}"/>
+  <xr:revisionPtr revIDLastSave="1293" documentId="8_{6055D0A3-676A-4D4D-A9E1-9A76BC3762E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02BCE1E5-D3ED-47F3-A00E-5FB2692EC511}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6F9A2E0A-FCD5-4099-AB1E-88BFB846A76D}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{6F9A2E0A-FCD5-4099-AB1E-88BFB846A76D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -867,32 +867,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFB773-84C8-4FDF-A3F8-2F632CD15839}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F72" zoomScale="95" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="L117" sqref="L4:L117"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="H84" sqref="H84:H114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" customWidth="1"/>
-    <col min="9" max="9" width="23.88671875" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>117</v>
       </c>
@@ -930,7 +930,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -968,7 +968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>31</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>32</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>33</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>34</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
         <v>35</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>36</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
         <v>37</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>38</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>39</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>40</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
         <v>41</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
         <v>42</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
         <v>43</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
         <v>44</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
         <v>45</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
         <v>46</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
         <v>47</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
         <v>48</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
         <v>49</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
         <v>50</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
         <v>51</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
         <v>52</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
         <v>53</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
         <v>54</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
         <v>55</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
         <v>56</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
         <v>57</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
         <v>58</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
         <v>59</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
         <v>60</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
         <v>61</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
         <v>62</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
         <v>63</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E66" t="s">
         <v>64</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E67" t="s">
         <v>65</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
         <v>66</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
         <v>67</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
         <v>68</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
         <v>69</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
         <v>70</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
         <v>71</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
         <v>72</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
         <v>73</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
         <v>74</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
         <v>75</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
         <v>76</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
         <v>77</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E80" t="s">
         <v>78</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E81" t="s">
         <v>79</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E82" t="s">
         <v>80</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E83" t="s">
         <v>81</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E84" t="s">
         <v>82</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="85" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E85" t="s">
         <v>83</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E86" t="s">
         <v>84</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E87" t="s">
         <v>85</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="88" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E88" t="s">
         <v>86</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E89" t="s">
         <v>87</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E90" t="s">
         <v>88</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E91" t="s">
         <v>89</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E92" t="s">
         <v>90</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E93" t="s">
         <v>91</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E94" t="s">
         <v>92</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E95" t="s">
         <v>93</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E96" t="s">
         <v>94</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E97" t="s">
         <v>95</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E98" t="s">
         <v>96</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="99" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E99" t="s">
         <v>97</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E100" t="s">
         <v>98</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E101" t="s">
         <v>99</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E102" t="s">
         <v>100</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E103" t="s">
         <v>101</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="104" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E104" t="s">
         <v>102</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E105" t="s">
         <v>103</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="106" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E106" t="s">
         <v>104</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E107" t="s">
         <v>105</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E108" t="s">
         <v>106</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="109" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E109" t="s">
         <v>107</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E110" t="s">
         <v>108</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="111" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E111" t="s">
         <v>109</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E112" t="s">
         <v>110</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="113" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E113" t="s">
         <v>111</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E114" t="s">
         <v>112</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E115" t="s">
         <v>113</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="5:12" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E116" t="s">
         <v>114</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E117" t="s">
         <v>121</v>
       </c>
@@ -4319,13 +4319,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L117" xr:uid="{A9EFB773-84C8-4FDF-A3F8-2F632CD15839}">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="FALSE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L117" xr:uid="{A9EFB773-84C8-4FDF-A3F8-2F632CD15839}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B1:D1048576">
     <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">

</xml_diff>

<commit_message>
Changing the names of some translation files to align with the number of sequences contained. Updating family iqtree files following new run.
</commit_message>
<xml_diff>
--- a/gene_review.xlsx
+++ b/gene_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1293" documentId="8_{6055D0A3-676A-4D4D-A9E1-9A76BC3762E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02BCE1E5-D3ED-47F3-A00E-5FB2692EC511}"/>
+  <xr:revisionPtr revIDLastSave="1301" documentId="8_{6055D0A3-676A-4D4D-A9E1-9A76BC3762E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD45B697-29FB-4A1E-9D9B-3778ADBFA097}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{6F9A2E0A-FCD5-4099-AB1E-88BFB846A76D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{6F9A2E0A-FCD5-4099-AB1E-88BFB846A76D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -867,32 +867,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EFB773-84C8-4FDF-A3F8-2F632CD15839}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="H84" sqref="H84:H114"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.68359375" customWidth="1"/>
+    <col min="2" max="2" width="10.68359375" customWidth="1"/>
+    <col min="3" max="3" width="16.26171875" customWidth="1"/>
+    <col min="4" max="4" width="17.83984375" customWidth="1"/>
+    <col min="5" max="5" width="17.68359375" customWidth="1"/>
+    <col min="6" max="6" width="17.578125" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.83984375" customWidth="1"/>
+    <col min="9" max="9" width="23.83984375" customWidth="1"/>
+    <col min="10" max="10" width="17.68359375" customWidth="1"/>
+    <col min="11" max="11" width="16.26171875" customWidth="1"/>
+    <col min="12" max="12" width="15.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>117</v>
       </c>
@@ -930,7 +930,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -968,7 +968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E33" t="s">
         <v>31</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E34" t="s">
         <v>32</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E35" t="s">
         <v>33</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E36" t="s">
         <v>34</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E37" t="s">
         <v>35</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E38" t="s">
         <v>36</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E39" t="s">
         <v>37</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E40" t="s">
         <v>38</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E41" t="s">
         <v>39</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E42" t="s">
         <v>40</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E43" t="s">
         <v>41</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E44" t="s">
         <v>42</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E45" t="s">
         <v>43</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E46" t="s">
         <v>44</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E47" t="s">
         <v>45</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E48" t="s">
         <v>46</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E49" t="s">
         <v>47</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E50" t="s">
         <v>48</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E51" t="s">
         <v>49</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E52" t="s">
         <v>50</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E53" t="s">
         <v>51</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E54" t="s">
         <v>52</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E55" t="s">
         <v>53</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E56" t="s">
         <v>54</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E57" t="s">
         <v>55</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E58" t="s">
         <v>56</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E59" t="s">
         <v>57</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E60" t="s">
         <v>58</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E61" t="s">
         <v>59</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E62" t="s">
         <v>60</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E63" t="s">
         <v>61</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E64" t="s">
         <v>62</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E65" t="s">
         <v>63</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E66" t="s">
         <v>64</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E67" t="s">
         <v>65</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E68" t="s">
         <v>66</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E69" t="s">
         <v>67</v>
       </c>
@@ -3070,7 +3070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E70" t="s">
         <v>68</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E71" t="s">
         <v>69</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E72" t="s">
         <v>70</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E73" t="s">
         <v>71</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E74" t="s">
         <v>72</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E75" t="s">
         <v>73</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E76" t="s">
         <v>74</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E77" t="s">
         <v>75</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E78" t="s">
         <v>76</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E79" t="s">
         <v>77</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E80" t="s">
         <v>78</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E81" t="s">
         <v>79</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E82" t="s">
         <v>80</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E83" t="s">
         <v>81</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E84" t="s">
         <v>82</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E85" t="s">
         <v>83</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E86" t="s">
         <v>84</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E87" t="s">
         <v>85</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E88" t="s">
         <v>86</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E89" t="s">
         <v>87</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E90" t="s">
         <v>88</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E91" t="s">
         <v>89</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E92" t="s">
         <v>90</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E93" t="s">
         <v>91</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E94" t="s">
         <v>92</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E95" t="s">
         <v>93</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E96" t="s">
         <v>94</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E97" t="s">
         <v>95</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E98" t="s">
         <v>96</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E99" t="s">
         <v>97</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E100" t="s">
         <v>98</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E101" t="s">
         <v>99</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E102" t="s">
         <v>100</v>
       </c>
@@ -3928,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E103" t="s">
         <v>101</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E104" t="s">
         <v>102</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E105" t="s">
         <v>103</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E106" t="s">
         <v>104</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E107" t="s">
         <v>105</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E108" t="s">
         <v>106</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E109" t="s">
         <v>107</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E110" t="s">
         <v>108</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E111" t="s">
         <v>109</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E112" t="s">
         <v>110</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E113" t="s">
         <v>111</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E114" t="s">
         <v>112</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E115" t="s">
         <v>113</v>
       </c>
@@ -4266,7 +4266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E116" t="s">
         <v>114</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="5:12" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="E117" t="s">
         <v>121</v>
       </c>
@@ -4319,7 +4319,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L117" xr:uid="{A9EFB773-84C8-4FDF-A3F8-2F632CD15839}"/>
+  <autoFilter ref="A1:L117" xr:uid="{A9EFB773-84C8-4FDF-A3F8-2F632CD15839}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B1:D1048576">
     <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
@@ -4351,5 +4357,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="41" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri"&amp;12&amp;KFF0000 OFFICIAL&amp;1#_x000D_</oddHeader>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;12&amp;KFF0000 OFFICIAL</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>